<commit_message>
Guidance on error handling where resource or operation not implemened. Fixes #208
</commit_message>
<xml_diff>
--- a/downloads/development/expected_error_codes.xlsx
+++ b/downloads/development/expected_error_codes.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\NHSDigital\gpconnect\downloads\development\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7335"/>
   </bookViews>
@@ -22,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="115">
   <si>
     <t>Scenario</t>
   </si>
@@ -361,13 +356,19 @@
   </si>
   <si>
     <t>FHIR validation invalid request - JSON (If invalid resource i.e. sending patient when it should be a practitioner)</t>
+  </si>
+  <si>
+    <t>FHIR Operation or Resource has not (yet) been implemented</t>
+  </si>
+  <si>
+    <t>NOT_IMPLEMENTED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +384,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -392,7 +399,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -450,11 +457,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -480,6 +498,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,8 +587,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C104" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:C104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C105" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:C105"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scenario" dataDxfId="0"/>
     <tableColumn id="2" name="Http Error Code"/>
@@ -619,7 +641,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -654,7 +676,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -863,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,6 +2148,17 @@
       </c>
       <c r="D104" s="1"/>
     </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" s="10">
+        <v>501</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Addition of NO_ORGANISATION_CONSENT error code to support PFS where a provider has disabled PFS for an organisation
</commit_message>
<xml_diff>
--- a/downloads/development/expected_error_codes.xlsx
+++ b/downloads/development/expected_error_codes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="117">
   <si>
     <t>Scenario</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>NOT_IMPLEMENTED</t>
+  </si>
+  <si>
+    <t>Returned by the Provider if a GP practice is not set up for patient access by any patient</t>
+  </si>
+  <si>
+    <t>NO_ORGANISATION_PFS</t>
   </si>
 </sst>
 </file>
@@ -587,8 +593,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C105" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:C105"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C106" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:C106"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scenario" dataDxfId="0"/>
     <tableColumn id="2" name="Http Error Code"/>
@@ -885,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,6 +2165,17 @@
         <v>114</v>
       </c>
     </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B106" s="10">
+        <v>403</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>